<commit_message>
removed the email feature as it's not needed and working on some ux updates
</commit_message>
<xml_diff>
--- a/payment_data.xlsx
+++ b/payment_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,30 +446,25 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Reason</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Reason</t>
+          <t>Amount</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Amount</t>
+          <t>Account Number</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Account Number</t>
+          <t>Account Name</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Account Name</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Bank Name</t>
         </is>
@@ -478,7 +473,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-05-17 21:55:14</t>
+          <t>2025-05-18 21:57</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -488,26 +483,21 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>&lt;mailto:gaiusnale@gmail.com|gaiusnale@gmail.com&gt;</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
           <t>Food</t>
         </is>
       </c>
+      <c r="D2" t="n">
+        <v>5000</v>
+      </c>
       <c r="E2" t="n">
-        <v>20000</v>
-      </c>
-      <c r="F2" t="n">
-        <v>2378492034</v>
+        <v>9055301016</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Gaius Omonale</t>
+        </is>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t>Gaius Omonale</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
         <is>
           <t>Opay</t>
         </is>

</xml_diff>

<commit_message>
now detecting that the user has filled out a form before and is asking for updated details
</commit_message>
<xml_diff>
--- a/payment_data.xlsx
+++ b/payment_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,30 +441,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>User ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Reason</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Account Number</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Account Name</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Bank Name</t>
         </is>
@@ -473,31 +478,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-05-18 21:57</t>
+          <t>2025-05-23 13:17</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gaius</t>
+          <t>U07EVCPHEMP</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Gaius Omonale</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Food</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>5000</v>
-      </c>
       <c r="E2" t="n">
-        <v>9055301016</v>
-      </c>
-      <c r="F2" t="inlineStr">
+        <v>6000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>7839920123</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>Gaius Omonale</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Opay</t>
         </is>

</xml_diff>

<commit_message>
creating production  mode for the slack bot
</commit_message>
<xml_diff>
--- a/payment_data.xlsx
+++ b/payment_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +513,44 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-05-23 14:00</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>U07EVCPHEMP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Gaius Omonale</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Yankee</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>50000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7839920123</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Gaius Omonale</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Opay</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>